<commit_message>
GROOVE experimentation of Maude case added
</commit_message>
<xml_diff>
--- a/papers/NaturalComputing/figs/cmsb.xlsx
+++ b/papers/NaturalComputing/figs/cmsb.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Papers\reaction-systems\papers\NaturalComputing\figs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rensink\Documents\Papers\reaction-systems\papers\NaturalComputing\figs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD36D61C-7F30-443A-AD1F-425C6F62F067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E948FCE-F285-44E5-8A00-A6C84BB9BE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -318,6 +318,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18045</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2101134</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2300038</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2359075</c:v>
+                </c:pt>
                 <c:pt idx="9">
                   <c:v>2410055</c:v>
                 </c:pt>
@@ -509,6 +524,7 @@
         <c:axId val="781143368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2500000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -567,7 +583,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:numFmt formatCode="#\ ###\ ##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -613,6 +629,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="781143368"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1564,7 +1581,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,6 +1610,9 @@
       <c r="C2">
         <v>0</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1604,6 +1624,9 @@
       <c r="C3">
         <v>716</v>
       </c>
+      <c r="D3">
+        <v>18045</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1659,6 +1682,9 @@
       <c r="C8">
         <v>6940</v>
       </c>
+      <c r="D8">
+        <v>2101134</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1670,6 +1696,9 @@
       <c r="C9">
         <v>1102</v>
       </c>
+      <c r="D9">
+        <v>2300038</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1680,6 +1709,9 @@
       </c>
       <c r="C10">
         <v>840</v>
+      </c>
+      <c r="D10">
+        <v>2359075</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excel with risks and states updated
</commit_message>
<xml_diff>
--- a/papers/NaturalComputing/figs/cmsb.xlsx
+++ b/papers/NaturalComputing/figs/cmsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rensink\Documents\Papers\reaction-systems\papers\NaturalComputing\figs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E948FCE-F285-44E5-8A00-A6C84BB9BE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6749C1CA-9B2F-46E1-A6AD-5055FDB4F31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16245" yWindow="0" windowWidth="12660" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -324,6 +324,18 @@
                 <c:pt idx="1">
                   <c:v>18045</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>145202</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>630986</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1444184</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1875086</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>2101134</c:v>
                 </c:pt>
@@ -413,6 +425,7 @@
         <c:axId val="566302880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="150000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1581,7 +1594,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D4" sqref="D4:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1638,6 +1651,9 @@
       <c r="C4">
         <v>8601</v>
       </c>
+      <c r="D4">
+        <v>145202</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1649,6 +1665,9 @@
       <c r="C5">
         <v>26582</v>
       </c>
+      <c r="D5">
+        <v>630986</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1660,6 +1679,9 @@
       <c r="C6">
         <v>37693</v>
       </c>
+      <c r="D6">
+        <v>1444184</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1670,6 +1692,9 @@
       </c>
       <c r="C7">
         <v>8100</v>
+      </c>
+      <c r="D7">
+        <v>1875086</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Spreadsheet updated: total state count and new state count now correct
</commit_message>
<xml_diff>
--- a/papers/NaturalComputing/figs/cmsb.xlsx
+++ b/papers/NaturalComputing/figs/cmsb.xlsx
@@ -5,27 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rensink\Documents\Papers\reaction-systems\papers\NaturalComputing\figs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Papers\reaction-systems\papers\NaturalComputing\figs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6749C1CA-9B2F-46E1-A6AD-5055FDB4F31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728B3A2C-9E46-4589-8146-A790724A95FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16245" yWindow="0" windowWidth="12660" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Depth</t>
   </si>
@@ -36,7 +47,10 @@
     <t>New risks</t>
   </si>
   <si>
-    <t>States</t>
+    <t>New states</t>
+  </si>
+  <si>
+    <t>Total states</t>
   </si>
 </sst>
 </file>
@@ -211,8 +225,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -293,7 +308,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>States</c:v>
+                  <c:v>Total states</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -321,32 +336,26 @@
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>18045</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>145202</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>630986</c:v>
+                  <c:v>126012</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1444184</c:v>
+                  <c:v>227866</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1875086</c:v>
+                  <c:v>248420</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2101134</c:v>
+                  <c:v>276924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2300038</c:v>
+                  <c:v>281854</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2359075</c:v>
+                  <c:v>286054</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2410055</c:v>
+                  <c:v>288854</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -355,6 +364,78 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-D1AB-4FFF-85E4-23F4D5776070}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>New states</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>126012</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>101854</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20554</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28504</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4930</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D29B-4EDC-9402-2B9255374430}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -426,6 +507,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="150000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -537,7 +619,7 @@
         <c:axId val="781143368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2500000"/>
+          <c:max val="300000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -1591,15 +1673,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1610,10 +1692,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1627,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -1637,11 +1722,12 @@
       <c r="C3">
         <v>716</v>
       </c>
-      <c r="D3">
-        <v>18045</v>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="0">D3-D2</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -1651,11 +1737,12 @@
       <c r="C4">
         <v>8601</v>
       </c>
-      <c r="D4">
-        <v>145202</v>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -1666,10 +1753,14 @@
         <v>26582</v>
       </c>
       <c r="D5">
-        <v>630986</v>
+        <v>126012</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>126012</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -1680,10 +1771,14 @@
         <v>37693</v>
       </c>
       <c r="D6">
-        <v>1444184</v>
+        <v>227866</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>101854</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -1694,10 +1789,14 @@
         <v>8100</v>
       </c>
       <c r="D7">
-        <v>1875086</v>
+        <v>248420</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>20554</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1708,10 +1807,14 @@
         <v>6940</v>
       </c>
       <c r="D8">
-        <v>2101134</v>
+        <v>276924</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>28504</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -1722,10 +1825,14 @@
         <v>1102</v>
       </c>
       <c r="D9">
-        <v>2300038</v>
+        <v>281854</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>4930</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11</v>
       </c>
@@ -1736,10 +1843,14 @@
         <v>840</v>
       </c>
       <c r="D10">
-        <v>2359075</v>
+        <v>286054</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>4200</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>12</v>
       </c>
@@ -1750,7 +1861,11 @@
         <v>560</v>
       </c>
       <c r="D11">
-        <v>2410055</v>
+        <v>288854</v>
+      </c>
+      <c r="E11">
+        <f>D11-D10</f>
+        <v>2800</v>
       </c>
     </row>
   </sheetData>
@@ -1795,14 +1910,6 @@
               <xm:sqref>D7</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Sheet1!B8:B8</xm:f>
-              <xm:sqref>D8</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!B9:B9</xm:f>
-              <xm:sqref>D9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
               <xm:f>Sheet1!B10:B10</xm:f>
               <xm:sqref>D10</xm:sqref>
             </x14:sparkline>
@@ -1812,6 +1919,38 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{3C4C7BD7-8AF1-45E8-B42F-E4EEB97BCF2D}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!B8:B8</xm:f>
+              <xm:sqref>D8</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{5B1E8935-1048-455D-B80E-F94E2B9207D1}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!B9:B9</xm:f>
+              <xm:sqref>D9</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Spreadsheet now in really correct version
</commit_message>
<xml_diff>
--- a/papers/NaturalComputing/figs/cmsb.xlsx
+++ b/papers/NaturalComputing/figs/cmsb.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Papers\reaction-systems\papers\NaturalComputing\figs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728B3A2C-9E46-4589-8146-A790724A95FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22AF4799-7B4B-461B-B7E4-9C718C871C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -164,38 +165,44 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>716</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>9317</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>35899</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>73591</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>81691</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>88631</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>89733</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>90573</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>91133</c:v>
                 </c:pt>
               </c:numCache>
@@ -239,38 +246,44 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:f>Sheet1!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>716</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>8601</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>26582</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>37693</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>8100</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>6940</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>1102</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>840</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>560</c:v>
                 </c:pt>
               </c:numCache>
@@ -329,32 +342,44 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:f>Sheet1!$D$2:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>769</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1345</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1873</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>8133</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42293</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>126012</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>227866</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>248420</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>276924</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>281854</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>286054</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>288854</c:v>
                 </c:pt>
               </c:numCache>
@@ -398,35 +423,44 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:f>Sheet1!$E$2:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>769</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>576</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>528</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>126012</c:v>
+                  <c:v>6260</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>34160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>83719</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>101854</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>20554</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>28504</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>4930</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>4200</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>2800</c:v>
                 </c:pt>
               </c:numCache>
@@ -1381,7 +1415,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1673,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1700,7 +1734,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1709,162 +1743,207 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>769</v>
+      </c>
+      <c r="E2">
+        <v>769</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>716</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>716</v>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1345</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E10" si="0">D3-D2</f>
-        <v>0</v>
+        <f t="shared" ref="E3:E12" si="0">D3-D2</f>
+        <v>576</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>9317</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>8601</v>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1873</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>528</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>35899</v>
+        <v>716</v>
       </c>
       <c r="C5">
-        <v>26582</v>
+        <v>716</v>
       </c>
       <c r="D5">
-        <v>126012</v>
+        <v>8133</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>126012</v>
+        <v>6260</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>73591</v>
+        <v>9317</v>
       </c>
       <c r="C6">
-        <v>37693</v>
+        <v>8601</v>
       </c>
       <c r="D6">
-        <v>227866</v>
+        <v>42293</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>101854</v>
+        <v>34160</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>81691</v>
+        <v>35899</v>
       </c>
       <c r="C7">
-        <v>8100</v>
+        <v>26582</v>
       </c>
       <c r="D7">
-        <v>248420</v>
+        <v>126012</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>20554</v>
+        <v>83719</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>88631</v>
+        <v>73591</v>
       </c>
       <c r="C8">
-        <v>6940</v>
+        <v>37693</v>
       </c>
       <c r="D8">
-        <v>276924</v>
+        <v>227866</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>28504</v>
+        <v>101854</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>89733</v>
+        <v>81691</v>
       </c>
       <c r="C9">
-        <v>1102</v>
+        <v>8100</v>
       </c>
       <c r="D9">
-        <v>281854</v>
+        <v>248420</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>4930</v>
+        <v>20554</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>90573</v>
+        <v>88631</v>
       </c>
       <c r="C10">
-        <v>840</v>
+        <v>6940</v>
       </c>
       <c r="D10">
-        <v>286054</v>
+        <v>276924</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>4200</v>
+        <v>28504</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>89733</v>
+      </c>
+      <c r="C11">
+        <v>1102</v>
+      </c>
+      <c r="D11">
+        <v>281854</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>4930</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>90573</v>
+      </c>
+      <c r="C12">
+        <v>840</v>
+      </c>
+      <c r="D12">
+        <v>286054</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B13">
         <v>91133</v>
       </c>
-      <c r="C11">
+      <c r="C13">
         <v>560</v>
       </c>
-      <c r="D11">
+      <c r="D13">
         <v>288854</v>
       </c>
-      <c r="E11">
-        <f>D11-D10</f>
+      <c r="E13">
+        <f>D13-D12</f>
         <v>2800</v>
       </c>
     </row>
@@ -1875,7 +1954,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{054E05DF-61C0-4DA0-B962-09FBDE170577}">
+        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="gap" xr2:uid="{054E05DF-61C0-4DA0-B962-09FBDE170577}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1885,14 +1964,6 @@
           <x14:colorHigh rgb="FFD00000"/>
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!B2:B2</xm:f>
-              <xm:sqref>D2</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!B3:B3</xm:f>
-              <xm:sqref>D3</xm:sqref>
-            </x14:sparkline>
             <x14:sparkline>
               <xm:f>Sheet1!B4:B4</xm:f>
               <xm:sqref>D4</xm:sqref>
@@ -1910,16 +1981,24 @@
               <xm:sqref>D7</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Sheet1!B10:B10</xm:f>
-              <xm:sqref>D10</xm:sqref>
+              <xm:f>Sheet1!B8:B8</xm:f>
+              <xm:sqref>D8</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
-              <xm:f>Sheet1!B11:B11</xm:f>
-              <xm:sqref>D11</xm:sqref>
+              <xm:f>Sheet1!B9:B9</xm:f>
+              <xm:sqref>D9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B12:B12</xm:f>
+              <xm:sqref>D12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B13:B13</xm:f>
+              <xm:sqref>D13</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{3C4C7BD7-8AF1-45E8-B42F-E4EEB97BCF2D}">
+        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="gap" xr2:uid="{3C4C7BD7-8AF1-45E8-B42F-E4EEB97BCF2D}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1930,12 +2009,12 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!B8:B8</xm:f>
-              <xm:sqref>D8</xm:sqref>
+              <xm:f>Sheet1!B10:B10</xm:f>
+              <xm:sqref>D10</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{5B1E8935-1048-455D-B80E-F94E2B9207D1}">
+        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="gap" xr2:uid="{5B1E8935-1048-455D-B80E-F94E2B9207D1}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1946,8 +2025,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!B9:B9</xm:f>
-              <xm:sqref>D9</xm:sqref>
+              <xm:f>Sheet1!B11:B11</xm:f>
+              <xm:sqref>D11</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>